<commit_message>
Do more tests with fixed length window
</commit_message>
<xml_diff>
--- a/distances/by_vowel_diff_oldnew.xlsx
+++ b/distances/by_vowel_diff_oldnew.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="280" yWindow="460" windowWidth="23220" windowHeight="17540"/>
+    <workbookView xWindow="15980" yWindow="460" windowWidth="12740" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="by_vowel_diff_oldnew" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="30">
   <si>
     <t>pulm_2</t>
   </si>
@@ -96,19 +96,25 @@
     <t>('s08', 'question', 'coronal', 'o')</t>
   </si>
   <si>
-    <t>fixed_length</t>
-  </si>
-  <si>
-    <t>diff(fixed-new)</t>
-  </si>
-  <si>
-    <t>diff(fixed-old)</t>
+    <t>diff(fixed_mean-new)</t>
+  </si>
+  <si>
+    <t>diff(fixed_mean-old)</t>
+  </si>
+  <si>
+    <t>fixed_mean</t>
+  </si>
+  <si>
+    <t>fixed_qu1</t>
+  </si>
+  <si>
+    <t>diff(qu1-mean)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -245,7 +251,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +429,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -586,9 +598,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -943,11 +956,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -955,12 +968,15 @@
     <col min="1" max="2" width="9.83203125" customWidth="1"/>
     <col min="3" max="3" width="24" customWidth="1"/>
     <col min="4" max="4" width="16.1640625" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="16" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="0.1640625" customWidth="1"/>
+    <col min="11" max="11" width="15.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -983,16 +999,22 @@
         <v>6</v>
       </c>
       <c r="H1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I1" t="s">
         <v>25</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>26</v>
       </c>
-      <c r="J1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1025,8 +1047,15 @@
         <f>H2-E2</f>
         <v>-9.0515545650000639E-3</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K2">
+        <v>0.84612357339599997</v>
+      </c>
+      <c r="L2">
+        <f>K2-H2</f>
+        <v>3.8961038961000005E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1059,8 +1088,15 @@
         <f t="shared" ref="J3:J30" si="1">H3-E3</f>
         <v>-2.2417153950999968E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K3">
+        <v>0.84186159844099995</v>
+      </c>
+      <c r="L3">
+        <f t="shared" ref="L3:L30" si="2">K3-H3</f>
+        <v>-2.923976608000034E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -1093,8 +1129,15 @@
         <f t="shared" si="1"/>
         <v>0.19940476147599995</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K4">
+        <v>0.77261904761900002</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="2"/>
+        <v>5.089285714300007E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -1127,8 +1170,15 @@
         <f t="shared" si="1"/>
         <v>0.45092226602399998</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K5">
+        <v>0.88438735177899996</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="2"/>
+        <v>5.9288537549999631E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1161,8 +1211,15 @@
         <f t="shared" si="1"/>
         <v>1.7942584072000001E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K6">
+        <v>0.97368421052599996</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="2"/>
+        <v>4.5454545453999962E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -1195,8 +1252,15 @@
         <f t="shared" si="1"/>
         <v>1.1570248273000017E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K7">
+        <v>0.99421487603299996</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="2"/>
+        <v>1.6942148759999998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1229,8 +1293,15 @@
         <f t="shared" si="1"/>
         <v>0.54931972742200008</v>
       </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K8">
+        <v>0.941326530612</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="2"/>
+        <v>-2.3809523810000011E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1263,15 +1334,22 @@
         <f t="shared" si="1"/>
         <v>0.21159420244900007</v>
       </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" t="s">
+      <c r="K9">
+        <v>0.94347826086999997</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="2"/>
+        <v>3.7681159420999921E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D10">
@@ -1297,15 +1375,22 @@
         <f t="shared" si="1"/>
         <v>-7.3099414748999947E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="K10">
+        <v>0.86549707602299997</v>
+      </c>
+      <c r="L10">
+        <f t="shared" si="2"/>
+        <v>6.1403508771999959E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D11">
@@ -1331,8 +1416,15 @@
         <f t="shared" si="1"/>
         <v>3.5714285570999982E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K11">
+        <v>0.72321428571400004</v>
+      </c>
+      <c r="L11">
+        <f t="shared" si="2"/>
+        <v>0.10714285714300009</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1365,8 +1457,15 @@
         <f t="shared" si="1"/>
         <v>8.9285709999999963E-3</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>7</v>
       </c>
@@ -1399,8 +1498,15 @@
         <f t="shared" si="1"/>
         <v>0.41964285714299998</v>
       </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K13">
+        <v>0.86607142857099995</v>
+      </c>
+      <c r="L13">
+        <f t="shared" si="2"/>
+        <v>8.9285714279999651E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -1433,8 +1539,15 @@
         <f t="shared" si="1"/>
         <v>0.51190476223799997</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K14">
+        <v>0.88095238095200001</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>3.5714285714000038E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>7</v>
       </c>
@@ -1467,8 +1580,15 @@
         <f t="shared" si="1"/>
         <v>0.22619047614299997</v>
       </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K15">
+        <v>0.63095238095200001</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="2"/>
+        <v>2.3809523809000033E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>7</v>
       </c>
@@ -1501,8 +1621,15 @@
         <f t="shared" si="1"/>
         <v>0.27380952361900002</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K16">
+        <v>0.82142857142900005</v>
+      </c>
+      <c r="L16">
+        <f t="shared" si="2"/>
+        <v>2.3809523810000011E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>7</v>
       </c>
@@ -1535,8 +1662,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K17">
+        <v>1</v>
+      </c>
+      <c r="L17">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -1569,8 +1703,15 @@
         <f t="shared" si="1"/>
         <v>-4.7619047475999987E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K18">
+        <v>0.80952380952400005</v>
+      </c>
+      <c r="L18">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -1603,8 +1744,15 @@
         <f t="shared" si="1"/>
         <v>0.625</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K19">
+        <v>1</v>
+      </c>
+      <c r="L19">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1637,8 +1785,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K20">
+        <v>1</v>
+      </c>
+      <c r="L20">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1671,8 +1826,15 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K21">
+        <v>1</v>
+      </c>
+      <c r="L21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1705,8 +1867,15 @@
         <f t="shared" si="1"/>
         <v>0.428571429</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K22">
+        <v>1</v>
+      </c>
+      <c r="L22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -1739,8 +1908,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1773,8 +1949,15 @@
         <f t="shared" si="1"/>
         <v>0.85714285700000004</v>
       </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>8</v>
       </c>
@@ -1807,8 +1990,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K25">
+        <v>1</v>
+      </c>
+      <c r="L25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1841,8 +2031,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>7</v>
       </c>
@@ -1875,8 +2072,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K27">
+        <v>1</v>
+      </c>
+      <c r="L27">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1909,8 +2113,15 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K28">
+        <v>1</v>
+      </c>
+      <c r="L28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>7</v>
       </c>
@@ -1943,8 +2154,15 @@
         <f t="shared" si="1"/>
         <v>0.25</v>
       </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K29">
+        <v>1</v>
+      </c>
+      <c r="L29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1977,9 +2195,26 @@
         <f t="shared" si="1"/>
         <v>-0.5</v>
       </c>
+      <c r="K30">
+        <v>0.5</v>
+      </c>
+      <c r="L30">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="G2:G30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I30">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -1989,7 +2224,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I2:I30">
+  <conditionalFormatting sqref="J2:J30">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -1999,7 +2234,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J30">
+  <conditionalFormatting sqref="F2:F30">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -2009,7 +2244,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F2:F30">
+  <conditionalFormatting sqref="L2:L30">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>